<commit_message>
Update: Missing connection and via placement
</commit_message>
<xml_diff>
--- a/PaHoy/Production/Bill of Materials-PaHoy(JLC_PCB_Assembly).xlsx
+++ b/PaHoy/Production/Bill of Materials-PaHoy(JLC_PCB_Assembly).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mblank\Desktop\Stuff\AltiumTests\PaHoy\PaHoy\Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{852F716B-D58B-4B7B-BA7A-31509D9240AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B60EEBDB-3DB4-419E-B23B-569214C7D202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="8330" xr2:uid="{366F54DC-867C-47A6-980E-64C815BEC6E1}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="8330" xr2:uid="{45A1AB3A-FA11-49BD-A0FE-43D407179F75}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-PaHoy(JLC_PCB" sheetId="1" r:id="rId1"/>
@@ -623,7 +623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA823D7-4886-43C1-87C6-6DC0FC9638F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019F5F3B-4E58-4414-B5DF-9C1242D54F37}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>